<commit_message>
First version with multiplayer ready skills
</commit_message>
<xml_diff>
--- a/DotT Plan.xlsx
+++ b/DotT Plan.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Epic Plan" sheetId="1" r:id="rId1"/>
     <sheet name="Skill requirements" sheetId="4" r:id="rId2"/>
-    <sheet name="Sayfa1" sheetId="2" r:id="rId3"/>
+    <sheet name="weird berke numbers" sheetId="2" r:id="rId3"/>
+    <sheet name="Anatomy of a hero" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
   <si>
     <t>Lobby</t>
   </si>
@@ -182,6 +183,72 @@
   </si>
   <si>
     <t>use &gt; damage/heal(target,self,area)</t>
+  </si>
+  <si>
+    <t>DEPRECATED - refer to "Skill requirements.txt" for further info</t>
+  </si>
+  <si>
+    <t>Local Player Master</t>
+  </si>
+  <si>
+    <t>Actual Hero Object</t>
+  </si>
+  <si>
+    <t>Player Network Events Handler</t>
+  </si>
+  <si>
+    <t>War Fog Controller</t>
+  </si>
+  <si>
+    <t>Skill Controller</t>
+  </si>
+  <si>
+    <t>Hero gfx</t>
+  </si>
+  <si>
+    <t>Nav Mesh Agent</t>
+  </si>
+  <si>
+    <t>Hero Object Relay</t>
+  </si>
+  <si>
+    <t>Object Pool (for basic attacks)</t>
+  </si>
+  <si>
+    <t>&gt; childs</t>
+  </si>
+  <si>
+    <t>Skill Master objects</t>
+  </si>
+  <si>
+    <t>e.g. Q Skill</t>
+  </si>
+  <si>
+    <t>Hero Object</t>
+  </si>
+  <si>
+    <t>has public refs for &lt;</t>
+  </si>
+  <si>
+    <t>only server got the refs</t>
+  </si>
+  <si>
+    <t>Remember that everything other that the inputs are handled by the server</t>
+  </si>
+  <si>
+    <t>&gt; these will come with their own pools</t>
+  </si>
+  <si>
+    <t>&gt;  childs</t>
+  </si>
+  <si>
+    <t>Telegraph object</t>
+  </si>
+  <si>
+    <t>&gt;childs</t>
+  </si>
+  <si>
+    <t>TriggerChild</t>
   </si>
 </sst>
 </file>
@@ -369,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -430,6 +497,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,7 +792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -902,7 +981,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1072,6 +1151,9 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
+      <c r="F12" s="17" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="4"/>
@@ -1491,4 +1573,235 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="1"/>
+    <col min="7" max="7" width="17.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" style="1"/>
+    <col min="9" max="9" width="4.28515625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="18.5703125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="19"/>
+      <c r="H2" s="18"/>
+      <c r="L2" s="17"/>
+    </row>
+    <row r="3" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="3:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="3:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a few utilities. Added the UML Diagram
</commit_message>
<xml_diff>
--- a/DotT Plan.xlsx
+++ b/DotT Plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity\_DotT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity\2018\_DotT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
   </bookViews>
   <sheets>
     <sheet name="Epic Plan" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
   <si>
     <t>Lobby</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>Nexus Controller</t>
-  </si>
-  <si>
-    <t>Base Controller</t>
   </si>
   <si>
     <t>Pooling Controller</t>
@@ -302,7 +299,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -432,11 +429,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -489,6 +495,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -498,17 +516,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -792,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -810,21 +819,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="24" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="19"/>
+      <c r="B2" s="23"/>
       <c r="D2" s="5"/>
       <c r="E2" s="4"/>
-      <c r="H2" s="19"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
@@ -835,7 +844,7 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>9</v>
@@ -931,16 +940,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
-      <c r="H10" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="D11" s="3"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
@@ -999,100 +1009,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
-        <v>35</v>
+      <c r="B1" s="22" t="s">
+        <v>34</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
-      <c r="H1" s="20" t="s">
-        <v>36</v>
+      <c r="H1" s="24" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="19"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="H2" s="18"/>
+      <c r="H2" s="22"/>
       <c r="L2" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="15"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="15"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="15"/>
@@ -1105,7 +1115,7 @@
     </row>
     <row r="8" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -1118,7 +1128,7 @@
     </row>
     <row r="9" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1141,7 +1151,7 @@
     </row>
     <row r="11" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1152,7 +1162,7 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1210,25 +1220,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1579,7 +1589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -1598,28 +1608,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
-        <v>53</v>
+      <c r="B1" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="20"/>
+      <c r="E1" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="19"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="19"/>
-      <c r="H2" s="18"/>
+      <c r="E2" s="23"/>
+      <c r="H2" s="22"/>
       <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>24</v>
@@ -1629,7 +1639,7 @@
         <v>23</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -1638,17 +1648,17 @@
     </row>
     <row r="4" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -1664,20 +1674,20 @@
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>69</v>
+        <v>63</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>68</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>21</v>
@@ -1685,11 +1695,11 @@
       <c r="C6" s="4"/>
       <c r="D6" s="15"/>
       <c r="E6" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="24" t="s">
-        <v>70</v>
+      <c r="G6" s="21" t="s">
+        <v>69</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -1701,41 +1711,41 @@
       <c r="C7" s="4"/>
       <c r="D7" s="15"/>
       <c r="E7" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="22" t="s">
-        <v>56</v>
+      <c r="B8" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="23"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="21" t="s">
-        <v>57</v>
+      <c r="B9" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>

</xml_diff>